<commit_message>
1. Latest xls push.
</commit_message>
<xml_diff>
--- a/cordexp/models/ipsl-wrf381p/cordexp_eur_11_ipsl_wrf381p_atmos.xlsx
+++ b/cordexp/models/ipsl-wrf381p/cordexp_eur_11_ipsl_wrf381p_atmos.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvautard\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -19,12 +24,12 @@
     <sheet name="8. Gravity Waves" sheetId="10" r:id="rId10"/>
     <sheet name="9. Natural Forcing" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="1042">
   <si>
     <t>ES-DOC CORDEX Model Documentation</t>
   </si>
@@ -3084,13 +3089,81 @@
   </si>
   <si>
     <t>stratospheric aerosols optical thickness</t>
+  </si>
+  <si>
+    <t>Institute Pierre-Simon Laplace</t>
+  </si>
+  <si>
+    <t>No development but application of the WRF model to Euro-Cordex</t>
+  </si>
+  <si>
+    <t>Weather Research and Forecasting (WRF) model</t>
+  </si>
+  <si>
+    <t>Frome the WRF website https://www.mmm.ucar.edu/weather-research-and-forecasting-model : "The Weather Research and Forecasting (WRF) Model is a next-generation mesoscale numerical weather prediction system designed for both atmospheric research and operational forecasting applications. It features two dynamical cores, a data assimilation system, and a software architecture supporting parallel computation and system extensibility. The model serves a wide range of meteorological applications across scales from tens of meters to thousands of kilometers. The effort to develop WRF began in the latter 1990's and was a collaborative partnership of the National Center for Atmospheric Research (NCAR), the National Oceanic and Atmospheric Administration (represented by the National Centers for Environmental Prediction (NCEP) and the Earth System Research Laboratory), the U.S. Air Force, the Naval Research Laboratory, the University of Oklahoma, and the Federal Aviation Administration (FAA).
+For researchers, WRF can produce simulations based on actual atmospheric conditions (i.e., from observations and analyses) or idealized conditions. WRF offers operational forecasting a flexible and computationally-efficient platform, while reflecting recent advances in physics, numerics, and data assimilation contributed by developers from the expansive research community. WRF is currently in operational use at NCEP and other national meteorological centers as well as in real-time forecasting configurations at laboratories, universities, and companies.
+WRF has a large worldwide community of registered users (a cumulative total of over 48,000 in over 160 countries), and NCAR provides regular workshops and tutorials on it. The WRF system contains two dynamical solvers, referred to as the ARW (Advanced Research WRF) core and the NMM (Nonhydrostatic Mesoscale Model) core. The ARW has been developed in large part and is maintained by NCAR's Mesoscale and Microscale Meteorology Laboratory, and its users' page is: WRF-ARW Users' Page. The NMM core was developed by the National Centers for Environmental Prediction (NCEP), and is currently used in their HWRF (Hurricane WRF) system."</t>
+  </si>
+  <si>
+    <t>0.11x0.11 degrees rotated lat-lon</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>The model has been tuned by testing a number of combinations of microphysics and convection schemes and checking seasonal average temperature and precipitation at 50 km resolution over 5 years against EOBS. No other tuning performed.</t>
+  </si>
+  <si>
+    <t>Bias of seasonal temperature and precipitation</t>
+  </si>
+  <si>
+    <t>No trend tuning</t>
+  </si>
+  <si>
+    <t>Rotated lat-lon 0.11x0.11 grid</t>
+  </si>
+  <si>
+    <t>Rotated pole: longitude : -162 ; latitude: 39.25</t>
+  </si>
+  <si>
+    <t>0.11°</t>
+  </si>
+  <si>
+    <t>504 x 492</t>
+  </si>
+  <si>
+    <t>5 relaxation rows</t>
+  </si>
+  <si>
+    <t>494 x 482</t>
+  </si>
+  <si>
+    <t>WRF-ARW</t>
+  </si>
+  <si>
+    <t>RRTMG</t>
+  </si>
+  <si>
+    <t>New simplified Arakawa-Schubert</t>
+  </si>
+  <si>
+    <t>Included in Arakawa-Schubert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Thompson </t>
+  </si>
+  <si>
+    <t>As microphysics scheme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3191,6 +3264,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -3233,10 +3314,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3280,17 +3362,32 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3332,7 +3429,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3364,9 +3461,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3398,6 +3496,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3573,24 +3672,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -3598,7 +3699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3606,7 +3707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3614,7 +3715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -3622,7 +3723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -3630,47 +3731,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20.25">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="20.25">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="20.25">
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="20.25">
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="20.25">
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="20.25">
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="20.25">
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20.25">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="18">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
@@ -3678,7 +3779,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="18">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -3686,7 +3787,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="18">
       <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
@@ -3694,7 +3795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="18">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -3702,13 +3803,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="20.25">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="20.25">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -3724,12 +3825,12 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -3796,7 +3897,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="178" customHeight="1">
+    <row r="11" spans="1:29" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
@@ -4309,12 +4410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD77"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -4381,7 +4484,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -4709,7 +4812,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:29" ht="178" customHeight="1">
+    <row r="73" spans="1:29" ht="177.95" customHeight="1">
       <c r="B73" s="11"/>
     </row>
     <row r="75" spans="1:29" ht="24" customHeight="1">
@@ -4752,8 +4855,8 @@
       <formula1>AA28:AB28</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
       <formula1>AA44:AB44</formula1>
@@ -4776,19 +4879,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="80.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
@@ -4799,7 +4904,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18">
       <c r="A5" s="9" t="s">
         <v>31</v>
       </c>
@@ -4815,7 +4920,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="10" t="s">
         <v>34</v>
       </c>
@@ -4823,18 +4928,26 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="18">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4843,7 +4956,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="15.75">
       <c r="A16" s="10" t="s">
         <v>34</v>
       </c>
@@ -4851,7 +4964,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="18">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
     </row>
@@ -4873,12 +4986,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG93"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -4919,7 +5034,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1022</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -4972,8 +5089,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
+    <row r="16" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B16" s="16" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="18" spans="1:33" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
@@ -4995,7 +5114,9 @@
       </c>
     </row>
     <row r="20" spans="1:33" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>63</v>
       </c>
@@ -5031,7 +5152,9 @@
       </c>
     </row>
     <row r="25" spans="1:33" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="AA25" s="6" t="s">
         <v>70</v>
       </c>
@@ -5087,7 +5210,9 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="B33" s="11"/>
+      <c r="B33" s="11" t="s">
+        <v>1024</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
       <c r="A35" s="9" t="s">
@@ -5109,7 +5234,9 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
-      <c r="B37" s="11"/>
+      <c r="B37" s="11">
+        <v>32</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
       <c r="A39" s="9" t="s">
@@ -5131,7 +5258,9 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
-      <c r="B41" s="11"/>
+      <c r="B41" s="11" t="s">
+        <v>1025</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1">
       <c r="A44" s="12" t="s">
@@ -5166,7 +5295,9 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="24" customHeight="1">
-      <c r="B49" s="11"/>
+      <c r="B49" s="11">
+        <v>60</v>
+      </c>
     </row>
     <row r="51" spans="1:3" ht="24" customHeight="1">
       <c r="A51" s="9" t="s">
@@ -5188,7 +5319,14 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="24" customHeight="1">
-      <c r="B53" s="11"/>
+      <c r="B53" s="11">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54">
+        <v>900</v>
+      </c>
     </row>
     <row r="55" spans="1:3" ht="24" customHeight="1">
       <c r="A55" s="9" t="s">
@@ -5210,7 +5348,9 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="24" customHeight="1">
-      <c r="B57" s="11"/>
+      <c r="B57" s="11">
+        <v>900</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="24" customHeight="1">
       <c r="A60" s="12" t="s">
@@ -5245,7 +5385,9 @@
       </c>
     </row>
     <row r="65" spans="1:31" ht="24" customHeight="1">
-      <c r="B65" s="11"/>
+      <c r="B65" s="11" t="s">
+        <v>115</v>
+      </c>
       <c r="AA65" s="6" t="s">
         <v>115</v>
       </c>
@@ -5333,6 +5475,11 @@
         <v>131</v>
       </c>
     </row>
+    <row r="79" spans="1:31">
+      <c r="D79" s="6" t="s">
+        <v>1026</v>
+      </c>
+    </row>
     <row r="80" spans="1:31" ht="24" customHeight="1">
       <c r="A80" s="9" t="s">
         <v>132</v>
@@ -5357,8 +5504,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="178" customHeight="1">
-      <c r="B83" s="11"/>
+    <row r="83" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B83" s="11" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="85" spans="1:3" ht="24" customHeight="1">
       <c r="A85" s="9" t="s">
@@ -5385,7 +5534,9 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="24" customHeight="1">
-      <c r="B88" s="11"/>
+      <c r="B88" s="11" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="90" spans="1:3" ht="24" customHeight="1">
       <c r="A90" s="9" t="s">
@@ -5412,7 +5563,9 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
-      <c r="B93" s="11"/>
+      <c r="B93" s="11" t="s">
+        <v>1029</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="9">
@@ -5449,12 +5602,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -5521,8 +5676,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B11" s="11" t="s">
+        <v>1030</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
@@ -5557,7 +5714,9 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="AA19" s="6" t="s">
         <v>160</v>
       </c>
@@ -5591,7 +5750,9 @@
       </c>
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
-      <c r="B23" s="11"/>
+      <c r="B23" s="11" t="s">
+        <v>1031</v>
+      </c>
     </row>
     <row r="25" spans="1:30" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
@@ -5613,7 +5774,9 @@
       </c>
     </row>
     <row r="27" spans="1:30" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
+      <c r="B27" s="11" t="s">
+        <v>1032</v>
+      </c>
     </row>
     <row r="29" spans="1:30" ht="24" customHeight="1">
       <c r="A29" s="9" t="s">
@@ -5635,7 +5798,9 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
+      <c r="B31" s="11" t="s">
+        <v>1033</v>
+      </c>
     </row>
     <row r="33" spans="1:30" ht="24" customHeight="1">
       <c r="A33" s="9" t="s">
@@ -5657,7 +5822,9 @@
       </c>
     </row>
     <row r="35" spans="1:30" ht="24" customHeight="1">
-      <c r="B35" s="11"/>
+      <c r="B35" s="11" t="s">
+        <v>1034</v>
+      </c>
     </row>
     <row r="37" spans="1:30" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
@@ -5679,7 +5846,9 @@
       </c>
     </row>
     <row r="39" spans="1:30" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="s">
+        <v>1035</v>
+      </c>
     </row>
     <row r="41" spans="1:30" ht="24" customHeight="1">
       <c r="A41" s="9" t="s">
@@ -5701,7 +5870,9 @@
       </c>
     </row>
     <row r="43" spans="1:30" ht="24" customHeight="1">
-      <c r="B43" s="11"/>
+      <c r="B43" s="11" t="s">
+        <v>188</v>
+      </c>
       <c r="AA43" s="6" t="s">
         <v>187</v>
       </c>
@@ -5732,7 +5903,9 @@
       </c>
     </row>
     <row r="47" spans="1:30" ht="24" customHeight="1">
-      <c r="B47" s="11"/>
+      <c r="B47" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="AA47" s="6" t="s">
         <v>193</v>
       </c>
@@ -5834,7 +6007,9 @@
       </c>
     </row>
     <row r="59" spans="1:31" ht="24" customHeight="1">
-      <c r="B59" s="11"/>
+      <c r="B59" s="11" t="s">
+        <v>216</v>
+      </c>
       <c r="AA59" s="6" t="s">
         <v>215</v>
       </c>
@@ -5889,7 +6064,9 @@
       </c>
     </row>
     <row r="68" spans="1:32" ht="24" customHeight="1">
-      <c r="B68" s="11"/>
+      <c r="B68" s="11" t="s">
+        <v>228</v>
+      </c>
       <c r="AA68" s="6" t="s">
         <v>226</v>
       </c>
@@ -5938,12 +6115,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM104"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -5984,7 +6163,9 @@
       </c>
     </row>
     <row r="6" spans="1:36" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1036</v>
+      </c>
     </row>
     <row r="8" spans="1:36" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -6010,7 +6191,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="178" customHeight="1">
+    <row r="11" spans="1:36" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:36" ht="24" customHeight="1">
@@ -6033,7 +6214,9 @@
       </c>
     </row>
     <row r="15" spans="1:36" ht="24" customHeight="1">
-      <c r="B15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>252</v>
+      </c>
       <c r="AA15" s="6" t="s">
         <v>244</v>
       </c>
@@ -6252,7 +6435,9 @@
       </c>
     </row>
     <row r="44" spans="1:29" ht="24" customHeight="1">
-      <c r="B44" s="11"/>
+      <c r="B44" s="11" t="s">
+        <v>276</v>
+      </c>
       <c r="AA44" s="6" t="s">
         <v>276</v>
       </c>
@@ -6766,16 +6951,19 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD206"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AX218"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="B218" sqref="B218"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -6816,7 +7004,9 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1037</v>
+      </c>
     </row>
     <row r="8" spans="1:40" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -6842,7 +7032,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="178" customHeight="1">
+    <row r="11" spans="1:40" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:40" ht="24" customHeight="1">
@@ -6870,7 +7060,9 @@
       </c>
     </row>
     <row r="16" spans="1:40" ht="24" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>399</v>
+      </c>
       <c r="AA16" s="6" t="s">
         <v>394</v>
       </c>
@@ -6914,1650 +7106,2094 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="24" customHeight="1">
-      <c r="A19" s="12" t="s">
+    <row r="17" spans="1:40" ht="24" customHeight="1">
+      <c r="B17" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB17" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC17" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="AF17" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="AG17" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH17" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI17" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="AJ17" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="AL17" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="AM17" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="AN17" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" ht="24" customHeight="1">
+      <c r="B18" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="AA18" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB18" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC18" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="AF18" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="AG18" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH18" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI18" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="AJ18" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="AK18" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="AL18" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="AM18" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="AN18" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="24" customHeight="1">
+      <c r="B19" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="AA19" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB19" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC19" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="AF19" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="AG19" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH19" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI19" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="AJ19" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="AK19" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="AL19" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="AM19" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="AN19" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" ht="24" customHeight="1">
+      <c r="B20" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="AA20" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC20" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="AD20" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="AE20" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="AF20" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH20" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI20" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="AJ20" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="AK20" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="AL20" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="AM20" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="AN20" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" ht="24" customHeight="1">
+      <c r="A23" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B23" s="12" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="24" customHeight="1">
-      <c r="B20" s="13" t="s">
+    <row r="24" spans="1:40" ht="24" customHeight="1">
+      <c r="B24" s="13" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="24" customHeight="1">
-      <c r="A22" s="9" t="s">
+    <row r="26" spans="1:40" ht="24" customHeight="1">
+      <c r="A26" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B26" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="24" customHeight="1">
-      <c r="A23" s="14" t="s">
+    <row r="27" spans="1:40" ht="24" customHeight="1">
+      <c r="A27" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="24" customHeight="1">
-      <c r="B24" s="11"/>
-    </row>
-    <row r="26" spans="1:30" ht="24" customHeight="1">
-      <c r="A26" s="9" t="s">
+    <row r="28" spans="1:40" ht="24" customHeight="1">
+      <c r="B28" s="11"/>
+    </row>
+    <row r="30" spans="1:40" ht="24" customHeight="1">
+      <c r="A30" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="24" customHeight="1">
-      <c r="A27" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" ht="24" customHeight="1">
-      <c r="B28" s="11"/>
-      <c r="AA28" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="AB28" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="AC28" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="AD28" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" ht="24" customHeight="1">
-      <c r="A30" s="9" t="s">
-        <v>420</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" ht="24" customHeight="1">
+    <row r="31" spans="1:40" ht="24" customHeight="1">
       <c r="A31" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" ht="24" customHeight="1">
+      <c r="B32" s="11"/>
+      <c r="AA32" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="AB32" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="AC32" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="AD32" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" ht="24" customHeight="1">
+      <c r="A34" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" ht="24" customHeight="1">
+      <c r="A35" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C35" s="10" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="24" customHeight="1">
-      <c r="B32" s="10" t="s">
+    <row r="36" spans="1:32" ht="24" customHeight="1">
+      <c r="B36" s="10" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:32" ht="24" customHeight="1">
-      <c r="B33" s="11"/>
-      <c r="AA33" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="AB33" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="AC33" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="AD33" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="AE33" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="AF33" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:32" ht="24" customHeight="1">
-      <c r="A35" s="9" t="s">
-        <v>429</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="36" spans="1:32" ht="24" customHeight="1">
-      <c r="A36" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="24" customHeight="1">
       <c r="B37" s="11"/>
+      <c r="AA37" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="AB37" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="AC37" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="AD37" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AE37" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="AF37" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="39" spans="1:32" ht="24" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="40" spans="1:32" ht="24" customHeight="1">
       <c r="A40" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" ht="24" customHeight="1">
+      <c r="B41" s="11"/>
+    </row>
+    <row r="43" spans="1:32" ht="24" customHeight="1">
+      <c r="A43" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" ht="24" customHeight="1">
+      <c r="A44" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B44" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C44" s="10" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="41" spans="1:32" ht="24" customHeight="1">
-      <c r="B41" s="10" t="s">
+    <row r="45" spans="1:32" ht="24" customHeight="1">
+      <c r="B45" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:32" ht="24" customHeight="1">
-      <c r="B42" s="11"/>
-      <c r="AA42" s="6" t="s">
+    <row r="46" spans="1:32" ht="24" customHeight="1">
+      <c r="B46" s="11"/>
+      <c r="AA46" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="AB42" s="6" t="s">
+      <c r="AB46" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="AC42" s="6" t="s">
+      <c r="AC46" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:32" ht="24" customHeight="1">
-      <c r="A45" s="12" t="s">
+    <row r="49" spans="1:44" ht="24" customHeight="1">
+      <c r="A49" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B49" s="12" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="24" customHeight="1">
-      <c r="B46" s="13" t="s">
+    <row r="50" spans="1:44" ht="24" customHeight="1">
+      <c r="B50" s="13" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="48" spans="1:32" ht="24" customHeight="1">
-      <c r="A48" s="9" t="s">
+    <row r="52" spans="1:44" ht="24" customHeight="1">
+      <c r="A52" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B52" s="9" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="49" spans="1:50" ht="24" customHeight="1">
-      <c r="A49" s="14" t="s">
+    <row r="53" spans="1:44" ht="24" customHeight="1">
+      <c r="A53" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B53" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C53" s="10" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="50" spans="1:50" ht="24" customHeight="1">
-      <c r="B50" s="10" t="s">
+    <row r="54" spans="1:44" ht="24" customHeight="1">
+      <c r="B54" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:50" ht="24" customHeight="1">
-      <c r="B51" s="11"/>
-      <c r="AA51" s="6" t="s">
+    <row r="55" spans="1:44" ht="24" customHeight="1">
+      <c r="B55" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="AB51" s="6" t="s">
+      <c r="AA55" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB55" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="AC51" s="6" t="s">
+      <c r="AC55" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="AD51" s="6" t="s">
+      <c r="AD55" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="AE51" s="6" t="s">
+      <c r="AE55" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="AF51" s="6" t="s">
+      <c r="AF55" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="AG51" s="6" t="s">
+      <c r="AG55" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="AH51" s="6" t="s">
+      <c r="AH55" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="AI51" s="6" t="s">
+      <c r="AI55" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="AJ51" s="6" t="s">
+      <c r="AJ55" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="AK51" s="6" t="s">
+      <c r="AK55" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:50" ht="24" customHeight="1">
-      <c r="A53" s="9" t="s">
+    <row r="56" spans="1:44" ht="24" customHeight="1">
+      <c r="B56" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="AA56" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB56" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC56" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD56" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE56" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AF56" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG56" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH56" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI56" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ56" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK56" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:44" ht="24" customHeight="1">
+      <c r="B57" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA57" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB57" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC57" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD57" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE57" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AF57" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG57" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH57" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI57" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ57" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK57" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:44" ht="24" customHeight="1">
+      <c r="B58" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA58" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB58" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC58" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD58" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE58" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AF58" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG58" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH58" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI58" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ58" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK58" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:44" ht="24" customHeight="1">
+      <c r="B59" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="AA59" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB59" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC59" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD59" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE59" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AF59" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG59" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH59" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI59" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ59" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK59" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:44" ht="24" customHeight="1">
+      <c r="A61" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B61" s="9" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="54" spans="1:50" ht="24" customHeight="1">
-      <c r="A54" s="14" t="s">
+    <row r="62" spans="1:44" ht="24" customHeight="1">
+      <c r="A62" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B62" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C62" s="10" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="55" spans="1:50" ht="24" customHeight="1">
-      <c r="B55" s="10" t="s">
+    <row r="63" spans="1:44" ht="24" customHeight="1">
+      <c r="B63" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:50" ht="24" customHeight="1">
-      <c r="B56" s="11"/>
-      <c r="AA56" s="6" t="s">
+    <row r="64" spans="1:44" ht="24" customHeight="1">
+      <c r="B64" s="11"/>
+      <c r="AA64" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="AB56" s="6" t="s">
+      <c r="AB64" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="AC56" s="6" t="s">
+      <c r="AC64" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="AD56" s="6" t="s">
+      <c r="AD64" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="AE56" s="6" t="s">
+      <c r="AE64" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="AF56" s="6" t="s">
+      <c r="AF64" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="AG56" s="6" t="s">
+      <c r="AG64" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AH56" s="6" t="s">
+      <c r="AH64" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="AI56" s="6" t="s">
+      <c r="AI64" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="AJ56" s="6" t="s">
+      <c r="AJ64" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="AK56" s="6" t="s">
+      <c r="AK64" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AL56" s="6" t="s">
+      <c r="AL64" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="AM56" s="6" t="s">
+      <c r="AM64" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="AN56" s="6" t="s">
+      <c r="AN64" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="AO56" s="6" t="s">
+      <c r="AO64" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="AP56" s="6" t="s">
+      <c r="AP64" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AQ56" s="6" t="s">
+      <c r="AQ64" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="AR56" s="6" t="s">
+      <c r="AR64" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:50" ht="24" customHeight="1">
-      <c r="A58" s="9" t="s">
+    <row r="66" spans="1:50" ht="24" customHeight="1">
+      <c r="A66" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B66" s="9" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:50" ht="24" customHeight="1">
-      <c r="A59" s="14" t="s">
+    <row r="67" spans="1:50" ht="24" customHeight="1">
+      <c r="A67" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B67" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C67" s="10" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="60" spans="1:50" ht="24" customHeight="1">
-      <c r="B60" s="10" t="s">
+    <row r="68" spans="1:50" ht="24" customHeight="1">
+      <c r="B68" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:50" ht="24" customHeight="1">
-      <c r="B61" s="11"/>
-      <c r="AA61" s="6" t="s">
+    <row r="69" spans="1:50" ht="24" customHeight="1">
+      <c r="B69" s="11"/>
+      <c r="AA69" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="AB61" s="6" t="s">
+      <c r="AB69" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="AC61" s="6" t="s">
+      <c r="AC69" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="AD61" s="6" t="s">
+      <c r="AD69" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="AE61" s="6" t="s">
+      <c r="AE69" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="AF61" s="6" t="s">
+      <c r="AF69" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="AG61" s="6" t="s">
+      <c r="AG69" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="AH61" s="6" t="s">
+      <c r="AH69" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="AI61" s="6" t="s">
+      <c r="AI69" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="AJ61" s="6" t="s">
+      <c r="AJ69" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="AK61" s="6" t="s">
+      <c r="AK69" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="AL61" s="6" t="s">
+      <c r="AL69" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="AM61" s="6" t="s">
+      <c r="AM69" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="AN61" s="6" t="s">
+      <c r="AN69" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="AO61" s="6" t="s">
+      <c r="AO69" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="AP61" s="6" t="s">
+      <c r="AP69" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="AQ61" s="6" t="s">
+      <c r="AQ69" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="AR61" s="6" t="s">
+      <c r="AR69" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="AS61" s="6" t="s">
+      <c r="AS69" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="AT61" s="6" t="s">
+      <c r="AT69" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="AU61" s="6" t="s">
+      <c r="AU69" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="AV61" s="6" t="s">
+      <c r="AV69" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="AW61" s="6" t="s">
+      <c r="AW69" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="AX61" s="6" t="s">
+      <c r="AX69" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:50" ht="24" customHeight="1">
-      <c r="A64" s="12" t="s">
+    <row r="72" spans="1:50" ht="24" customHeight="1">
+      <c r="A72" s="12" t="s">
         <v>504</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B72" s="12" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="65" spans="1:34" ht="24" customHeight="1">
-      <c r="B65" s="13" t="s">
+    <row r="73" spans="1:50" ht="24" customHeight="1">
+      <c r="B73" s="13" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="67" spans="1:34" ht="24" customHeight="1">
-      <c r="A67" s="9" t="s">
+    <row r="75" spans="1:50" ht="24" customHeight="1">
+      <c r="A75" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B75" s="9" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="68" spans="1:34" ht="24" customHeight="1">
-      <c r="A68" s="14" t="s">
+    <row r="76" spans="1:50" ht="24" customHeight="1">
+      <c r="A76" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B76" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C76" s="10" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="69" spans="1:34" ht="24" customHeight="1">
-      <c r="B69" s="10" t="s">
+    <row r="77" spans="1:50" ht="24" customHeight="1">
+      <c r="B77" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:34" ht="24" customHeight="1">
-      <c r="B70" s="11"/>
-      <c r="AA70" s="6" t="s">
+    <row r="78" spans="1:50" ht="24" customHeight="1">
+      <c r="B78" s="11"/>
+      <c r="AA78" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="AB70" s="6" t="s">
+      <c r="AB78" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="AC70" s="6" t="s">
+      <c r="AC78" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="AD70" s="6" t="s">
+      <c r="AD78" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="AE70" s="6" t="s">
+      <c r="AE78" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="AF70" s="6" t="s">
+      <c r="AF78" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="AG70" s="6" t="s">
+      <c r="AG78" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="AH70" s="6" t="s">
+      <c r="AH78" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:34" ht="24" customHeight="1">
-      <c r="A72" s="9" t="s">
+    <row r="80" spans="1:50" ht="24" customHeight="1">
+      <c r="A80" s="9" t="s">
         <v>518</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B80" s="9" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="73" spans="1:34" ht="24" customHeight="1">
-      <c r="A73" s="14" t="s">
+    <row r="81" spans="1:32" ht="24" customHeight="1">
+      <c r="A81" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B81" s="10" t="s">
         <v>520</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C81" s="10" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="74" spans="1:34" ht="24" customHeight="1">
-      <c r="B74" s="10" t="s">
+    <row r="82" spans="1:32" ht="24" customHeight="1">
+      <c r="B82" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:34" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
-      <c r="AA75" s="6" t="s">
+    <row r="83" spans="1:32" ht="24" customHeight="1">
+      <c r="B83" s="11"/>
+      <c r="AA83" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="AB75" s="6" t="s">
+      <c r="AB83" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="AC75" s="6" t="s">
+      <c r="AC83" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="AD75" s="6" t="s">
+      <c r="AD83" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="AE75" s="6" t="s">
+      <c r="AE83" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="AF75" s="6" t="s">
+      <c r="AF83" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:34" ht="24" customHeight="1">
-      <c r="A78" s="12" t="s">
+    <row r="86" spans="1:32" ht="24" customHeight="1">
+      <c r="A86" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B86" s="12" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="79" spans="1:34" ht="24" customHeight="1">
-      <c r="B79" s="13" t="s">
+    <row r="87" spans="1:32" ht="24" customHeight="1">
+      <c r="B87" s="13" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="81" spans="1:31" ht="24" customHeight="1">
-      <c r="A81" s="9" t="s">
+    <row r="89" spans="1:32" ht="24" customHeight="1">
+      <c r="A89" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B89" s="9" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="82" spans="1:31" ht="24" customHeight="1">
-      <c r="A82" s="14" t="s">
+    <row r="90" spans="1:32" ht="24" customHeight="1">
+      <c r="A90" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B90" s="10" t="s">
         <v>531</v>
       </c>
-      <c r="C82" s="10" t="s">
+      <c r="C90" s="10" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="83" spans="1:31" ht="24" customHeight="1">
-      <c r="B83" s="10" t="s">
+    <row r="91" spans="1:32" ht="24" customHeight="1">
+      <c r="B91" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:31" ht="24" customHeight="1">
-      <c r="B84" s="11"/>
-      <c r="AA84" s="6" t="s">
+    <row r="92" spans="1:32" ht="24" customHeight="1">
+      <c r="B92" s="11"/>
+      <c r="AA92" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="AB84" s="6" t="s">
+      <c r="AB92" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="AC84" s="6" t="s">
+      <c r="AC92" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="AD84" s="6" t="s">
+      <c r="AD92" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="AE84" s="6" t="s">
+      <c r="AE92" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:31" ht="24" customHeight="1">
-      <c r="A86" s="9" t="s">
+    <row r="94" spans="1:32" ht="24" customHeight="1">
+      <c r="A94" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B94" s="9" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="87" spans="1:31" ht="24" customHeight="1">
-      <c r="A87" s="14" t="s">
+    <row r="95" spans="1:32" ht="24" customHeight="1">
+      <c r="A95" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B95" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="C87" s="10" t="s">
+      <c r="C95" s="10" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="88" spans="1:31" ht="24" customHeight="1">
-      <c r="B88" s="10" t="s">
+    <row r="96" spans="1:32" ht="24" customHeight="1">
+      <c r="B96" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="24" customHeight="1">
-      <c r="B89" s="11"/>
-      <c r="AA89" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="AB89" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="AC89" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="92" spans="1:31" ht="24" customHeight="1">
-      <c r="A92" s="12" t="s">
-        <v>540</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="93" spans="1:31" ht="24" customHeight="1">
-      <c r="B93" s="13" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="95" spans="1:31" ht="24" customHeight="1">
-      <c r="A95" s="9" t="s">
-        <v>543</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="96" spans="1:31" ht="24" customHeight="1">
-      <c r="A96" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B96" s="10" t="s">
-        <v>545</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="97" spans="1:33" ht="24" customHeight="1">
+    <row r="97" spans="1:30" ht="24" customHeight="1">
       <c r="B97" s="11"/>
       <c r="AA97" s="6" t="s">
-        <v>547</v>
+        <v>523</v>
       </c>
       <c r="AB97" s="6" t="s">
-        <v>548</v>
+        <v>525</v>
       </c>
       <c r="AC97" s="6" t="s">
-        <v>549</v>
-      </c>
-      <c r="AD97" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="100" spans="1:33" ht="24" customHeight="1">
+    <row r="100" spans="1:30" ht="24" customHeight="1">
       <c r="A100" s="12" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="101" spans="1:33" ht="24" customHeight="1">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="101" spans="1:30" ht="24" customHeight="1">
       <c r="B101" s="13" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="103" spans="1:33" ht="24" customHeight="1">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="103" spans="1:30" ht="24" customHeight="1">
       <c r="A103" s="9" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="104" spans="1:33" ht="24" customHeight="1">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="104" spans="1:30" ht="24" customHeight="1">
       <c r="A104" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B104" s="10" t="s">
+        <v>545</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="105" spans="1:30" ht="24" customHeight="1">
+      <c r="B105" s="11"/>
+      <c r="AA105" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="AB105" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="AC105" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="AD105" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="108" spans="1:30" ht="24" customHeight="1">
+      <c r="A108" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="109" spans="1:30" ht="24" customHeight="1">
+      <c r="B109" s="13" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="111" spans="1:30" ht="24" customHeight="1">
+      <c r="A111" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="112" spans="1:30" ht="24" customHeight="1">
+      <c r="A112" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B112" s="10" t="s">
         <v>554</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="C112" s="10" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="105" spans="1:33" ht="24" customHeight="1">
-      <c r="B105" s="10" t="s">
+    <row r="113" spans="1:33" ht="24" customHeight="1">
+      <c r="B113" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="106" spans="1:33" ht="24" customHeight="1">
-      <c r="B106" s="11"/>
-      <c r="AA106" s="6" t="s">
+    <row r="114" spans="1:33" ht="24" customHeight="1">
+      <c r="B114" s="11"/>
+      <c r="AA114" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="AB106" s="6" t="s">
+      <c r="AB114" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="AC106" s="6" t="s">
+      <c r="AC114" s="6" t="s">
         <v>558</v>
       </c>
-      <c r="AD106" s="6" t="s">
+      <c r="AD114" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="AE106" s="6" t="s">
+      <c r="AE114" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="AF106" s="6" t="s">
+      <c r="AF114" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="AG106" s="6" t="s">
+      <c r="AG114" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="108" spans="1:33" ht="24" customHeight="1">
-      <c r="A108" s="9" t="s">
+    <row r="116" spans="1:33" ht="24" customHeight="1">
+      <c r="A116" s="9" t="s">
         <v>562</v>
       </c>
-      <c r="B108" s="9" t="s">
+      <c r="B116" s="9" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="109" spans="1:33" ht="24" customHeight="1">
-      <c r="A109" s="14" t="s">
+    <row r="117" spans="1:33" ht="24" customHeight="1">
+      <c r="A117" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B109" s="10" t="s">
+      <c r="B117" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="C109" s="10" t="s">
+      <c r="C117" s="10" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="110" spans="1:33" ht="24" customHeight="1">
-      <c r="B110" s="10" t="s">
+    <row r="118" spans="1:33" ht="24" customHeight="1">
+      <c r="B118" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="111" spans="1:33" ht="24" customHeight="1">
-      <c r="B111" s="11"/>
-      <c r="AA111" s="6" t="s">
+    <row r="119" spans="1:33" ht="24" customHeight="1">
+      <c r="B119" s="11"/>
+      <c r="AA119" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="AB111" s="6" t="s">
+      <c r="AB119" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="AC111" s="6" t="s">
+      <c r="AC119" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="AD111" s="6" t="s">
+      <c r="AD119" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="AE111" s="6" t="s">
+      <c r="AE119" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="AF111" s="6" t="s">
+      <c r="AF119" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="114" spans="1:32" ht="24" customHeight="1">
-      <c r="A114" s="12" t="s">
+    <row r="122" spans="1:33" ht="24" customHeight="1">
+      <c r="A122" s="12" t="s">
         <v>565</v>
       </c>
-      <c r="B114" s="12" t="s">
+      <c r="B122" s="12" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="115" spans="1:32" ht="24" customHeight="1">
-      <c r="B115" s="13" t="s">
+    <row r="123" spans="1:33" ht="24" customHeight="1">
+      <c r="B123" s="13" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="117" spans="1:32" ht="24" customHeight="1">
-      <c r="A117" s="9" t="s">
+    <row r="125" spans="1:33" ht="24" customHeight="1">
+      <c r="A125" s="9" t="s">
         <v>568</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="B125" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:32" ht="24" customHeight="1">
-      <c r="A118" s="14" t="s">
+    <row r="126" spans="1:33" ht="24" customHeight="1">
+      <c r="A126" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B118" s="10" t="s">
+      <c r="B126" s="10" t="s">
         <v>569</v>
       </c>
-      <c r="C118" s="10" t="s">
+      <c r="C126" s="10" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="119" spans="1:32" ht="24" customHeight="1">
-      <c r="B119" s="11"/>
-    </row>
-    <row r="121" spans="1:32" ht="24" customHeight="1">
-      <c r="A121" s="9" t="s">
+    <row r="127" spans="1:33" ht="24" customHeight="1">
+      <c r="B127" s="11" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="129" spans="1:32" ht="24" customHeight="1">
+      <c r="A129" s="9" t="s">
         <v>571</v>
       </c>
-      <c r="B121" s="9" t="s">
+      <c r="B129" s="9" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="122" spans="1:32" ht="24" customHeight="1">
-      <c r="A122" s="14" t="s">
+    <row r="130" spans="1:32" ht="24" customHeight="1">
+      <c r="A130" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B122" s="10" t="s">
+      <c r="B130" s="10" t="s">
         <v>572</v>
       </c>
-      <c r="C122" s="10" t="s">
+      <c r="C130" s="10" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="123" spans="1:32" ht="24" customHeight="1">
-      <c r="B123" s="11"/>
-      <c r="AA123" s="6" t="s">
+    <row r="131" spans="1:32" ht="24" customHeight="1">
+      <c r="B131" s="11"/>
+      <c r="AA131" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="AB123" s="6" t="s">
+      <c r="AB131" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="AC123" s="6" t="s">
+      <c r="AC131" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="AD123" s="6" t="s">
+      <c r="AD131" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="125" spans="1:32" ht="24" customHeight="1">
-      <c r="A125" s="9" t="s">
+    <row r="133" spans="1:32" ht="24" customHeight="1">
+      <c r="A133" s="9" t="s">
         <v>574</v>
       </c>
-      <c r="B125" s="9" t="s">
+      <c r="B133" s="9" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="126" spans="1:32" ht="24" customHeight="1">
-      <c r="A126" s="14" t="s">
+    <row r="134" spans="1:32" ht="24" customHeight="1">
+      <c r="A134" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B126" s="10" t="s">
+      <c r="B134" s="10" t="s">
         <v>575</v>
       </c>
-      <c r="C126" s="10" t="s">
+      <c r="C134" s="10" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="127" spans="1:32" ht="24" customHeight="1">
-      <c r="B127" s="10" t="s">
+    <row r="135" spans="1:32" ht="24" customHeight="1">
+      <c r="B135" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:32" ht="24" customHeight="1">
-      <c r="B128" s="11"/>
-      <c r="AA128" s="6" t="s">
+    <row r="136" spans="1:32" ht="24" customHeight="1">
+      <c r="B136" s="11"/>
+      <c r="AA136" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="AB128" s="6" t="s">
+      <c r="AB136" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="AC128" s="6" t="s">
+      <c r="AC136" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="AD128" s="6" t="s">
+      <c r="AD136" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="AE128" s="6" t="s">
+      <c r="AE136" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="AF128" s="6" t="s">
+      <c r="AF136" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="130" spans="1:29" ht="24" customHeight="1">
-      <c r="A130" s="9" t="s">
+    <row r="138" spans="1:32" ht="24" customHeight="1">
+      <c r="A138" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="B130" s="9" t="s">
+      <c r="B138" s="9" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="131" spans="1:29" ht="24" customHeight="1">
-      <c r="A131" s="14" t="s">
+    <row r="139" spans="1:32" ht="24" customHeight="1">
+      <c r="A139" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B131" s="10" t="s">
+      <c r="B139" s="10" t="s">
         <v>578</v>
       </c>
-      <c r="C131" s="10" t="s">
+      <c r="C139" s="10" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="132" spans="1:29" ht="24" customHeight="1">
-      <c r="B132" s="11"/>
-    </row>
-    <row r="134" spans="1:29" ht="24" customHeight="1">
-      <c r="A134" s="9" t="s">
+    <row r="140" spans="1:32" ht="24" customHeight="1">
+      <c r="B140" s="11"/>
+    </row>
+    <row r="142" spans="1:32" ht="24" customHeight="1">
+      <c r="A142" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="B134" s="9" t="s">
+      <c r="B142" s="9" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="135" spans="1:29" ht="24" customHeight="1">
-      <c r="A135" s="14" t="s">
+    <row r="143" spans="1:32" ht="24" customHeight="1">
+      <c r="A143" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B135" s="10" t="s">
+      <c r="B143" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="C135" s="10" t="s">
+      <c r="C143" s="10" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="136" spans="1:29" ht="24" customHeight="1">
-      <c r="B136" s="10" t="s">
+    <row r="144" spans="1:32" ht="24" customHeight="1">
+      <c r="B144" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="1:29" ht="24" customHeight="1">
-      <c r="B137" s="11"/>
-      <c r="AA137" s="6" t="s">
+    <row r="145" spans="1:37" ht="24" customHeight="1">
+      <c r="B145" s="11"/>
+      <c r="AA145" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="AB137" s="6" t="s">
+      <c r="AB145" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="AC137" s="6" t="s">
+      <c r="AC145" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="140" spans="1:29" ht="24" customHeight="1">
-      <c r="A140" s="12" t="s">
+    <row r="148" spans="1:37" ht="24" customHeight="1">
+      <c r="A148" s="12" t="s">
         <v>582</v>
       </c>
-      <c r="B140" s="12" t="s">
+      <c r="B148" s="12" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="141" spans="1:29" ht="24" customHeight="1">
-      <c r="B141" s="13" t="s">
+    <row r="149" spans="1:37" ht="24" customHeight="1">
+      <c r="B149" s="13" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="143" spans="1:29" ht="24" customHeight="1">
-      <c r="A143" s="9" t="s">
+    <row r="151" spans="1:37" ht="24" customHeight="1">
+      <c r="A151" s="9" t="s">
         <v>585</v>
       </c>
-      <c r="B143" s="9" t="s">
+      <c r="B151" s="9" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="144" spans="1:29" ht="24" customHeight="1">
-      <c r="A144" s="14" t="s">
+    <row r="152" spans="1:37" ht="24" customHeight="1">
+      <c r="A152" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B144" s="10" t="s">
+      <c r="B152" s="10" t="s">
         <v>586</v>
       </c>
-      <c r="C144" s="10" t="s">
+      <c r="C152" s="10" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="145" spans="1:50" ht="24" customHeight="1">
-      <c r="B145" s="10" t="s">
+    <row r="153" spans="1:37" ht="24" customHeight="1">
+      <c r="B153" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="146" spans="1:50" ht="24" customHeight="1">
-      <c r="B146" s="11"/>
-      <c r="AA146" s="6" t="s">
+    <row r="154" spans="1:37" ht="24" customHeight="1">
+      <c r="B154" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="AB146" s="6" t="s">
+      <c r="AA154" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB154" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="AC146" s="6" t="s">
+      <c r="AC154" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="AD146" s="6" t="s">
+      <c r="AD154" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="AE146" s="6" t="s">
+      <c r="AE154" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="AF146" s="6" t="s">
+      <c r="AF154" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="AG146" s="6" t="s">
+      <c r="AG154" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="AH146" s="6" t="s">
+      <c r="AH154" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="AI146" s="6" t="s">
+      <c r="AI154" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="AJ146" s="6" t="s">
+      <c r="AJ154" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="AK146" s="6" t="s">
+      <c r="AK154" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="148" spans="1:50" ht="24" customHeight="1">
-      <c r="A148" s="9" t="s">
+    <row r="155" spans="1:37" ht="24" customHeight="1">
+      <c r="B155" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="AA155" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB155" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC155" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD155" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE155" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AF155" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG155" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH155" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI155" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ155" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK155" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="156" spans="1:37" ht="24" customHeight="1">
+      <c r="B156" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA156" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB156" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC156" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD156" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE156" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AF156" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG156" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH156" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI156" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ156" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK156" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="157" spans="1:37" ht="24" customHeight="1">
+      <c r="B157" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA157" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB157" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC157" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD157" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE157" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AF157" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG157" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH157" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI157" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ157" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK157" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="158" spans="1:37" ht="24" customHeight="1">
+      <c r="B158" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="AA158" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AB158" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC158" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD158" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE158" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AF158" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AG158" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH158" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI158" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AJ158" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AK158" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="160" spans="1:37" ht="24" customHeight="1">
+      <c r="A160" s="9" t="s">
         <v>588</v>
       </c>
-      <c r="B148" s="9" t="s">
+      <c r="B160" s="9" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="149" spans="1:50" ht="24" customHeight="1">
-      <c r="A149" s="14" t="s">
+    <row r="161" spans="1:50" ht="24" customHeight="1">
+      <c r="A161" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B149" s="10" t="s">
+      <c r="B161" s="10" t="s">
         <v>589</v>
       </c>
-      <c r="C149" s="10" t="s">
+      <c r="C161" s="10" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="150" spans="1:50" ht="24" customHeight="1">
-      <c r="B150" s="10" t="s">
+    <row r="162" spans="1:50" ht="24" customHeight="1">
+      <c r="B162" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="151" spans="1:50" ht="24" customHeight="1">
-      <c r="B151" s="11"/>
-      <c r="AA151" s="6" t="s">
+    <row r="163" spans="1:50" ht="24" customHeight="1">
+      <c r="B163" s="11"/>
+      <c r="AA163" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="AB151" s="6" t="s">
+      <c r="AB163" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="AC151" s="6" t="s">
+      <c r="AC163" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="AD151" s="6" t="s">
+      <c r="AD163" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="AE151" s="6" t="s">
+      <c r="AE163" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="AF151" s="6" t="s">
+      <c r="AF163" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="AG151" s="6" t="s">
+      <c r="AG163" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AH151" s="6" t="s">
+      <c r="AH163" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="AI151" s="6" t="s">
+      <c r="AI163" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="AJ151" s="6" t="s">
+      <c r="AJ163" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="AK151" s="6" t="s">
+      <c r="AK163" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AL151" s="6" t="s">
+      <c r="AL163" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="AM151" s="6" t="s">
+      <c r="AM163" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="AN151" s="6" t="s">
+      <c r="AN163" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="AO151" s="6" t="s">
+      <c r="AO163" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="AP151" s="6" t="s">
+      <c r="AP163" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AQ151" s="6" t="s">
+      <c r="AQ163" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="AR151" s="6" t="s">
+      <c r="AR163" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="153" spans="1:50" ht="24" customHeight="1">
-      <c r="A153" s="9" t="s">
+    <row r="165" spans="1:50" ht="24" customHeight="1">
+      <c r="A165" s="9" t="s">
         <v>591</v>
       </c>
-      <c r="B153" s="9" t="s">
+      <c r="B165" s="9" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="154" spans="1:50" ht="24" customHeight="1">
-      <c r="A154" s="14" t="s">
+    <row r="166" spans="1:50" ht="24" customHeight="1">
+      <c r="A166" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B154" s="10" t="s">
+      <c r="B166" s="10" t="s">
         <v>592</v>
       </c>
-      <c r="C154" s="10" t="s">
+      <c r="C166" s="10" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="155" spans="1:50" ht="24" customHeight="1">
-      <c r="B155" s="10" t="s">
+    <row r="167" spans="1:50" ht="24" customHeight="1">
+      <c r="B167" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="156" spans="1:50" ht="24" customHeight="1">
-      <c r="B156" s="11"/>
-      <c r="AA156" s="6" t="s">
+    <row r="168" spans="1:50" ht="24" customHeight="1">
+      <c r="B168" s="11"/>
+      <c r="AA168" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="AB156" s="6" t="s">
+      <c r="AB168" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="AC156" s="6" t="s">
+      <c r="AC168" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="AD156" s="6" t="s">
+      <c r="AD168" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="AE156" s="6" t="s">
+      <c r="AE168" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="AF156" s="6" t="s">
+      <c r="AF168" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="AG156" s="6" t="s">
+      <c r="AG168" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="AH156" s="6" t="s">
+      <c r="AH168" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="AI156" s="6" t="s">
+      <c r="AI168" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="AJ156" s="6" t="s">
+      <c r="AJ168" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="AK156" s="6" t="s">
+      <c r="AK168" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="AL156" s="6" t="s">
+      <c r="AL168" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="AM156" s="6" t="s">
+      <c r="AM168" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="AN156" s="6" t="s">
+      <c r="AN168" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="AO156" s="6" t="s">
+      <c r="AO168" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="AP156" s="6" t="s">
+      <c r="AP168" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="AQ156" s="6" t="s">
+      <c r="AQ168" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="AR156" s="6" t="s">
+      <c r="AR168" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="AS156" s="6" t="s">
+      <c r="AS168" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="AT156" s="6" t="s">
+      <c r="AT168" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="AU156" s="6" t="s">
+      <c r="AU168" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="AV156" s="6" t="s">
+      <c r="AV168" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="AW156" s="6" t="s">
+      <c r="AW168" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="AX156" s="6" t="s">
+      <c r="AX168" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="159" spans="1:50" ht="24" customHeight="1">
-      <c r="A159" s="12" t="s">
+    <row r="171" spans="1:50" ht="24" customHeight="1">
+      <c r="A171" s="12" t="s">
         <v>594</v>
       </c>
-      <c r="B159" s="12" t="s">
+      <c r="B171" s="12" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="160" spans="1:50" ht="24" customHeight="1">
-      <c r="B160" s="13" t="s">
+    <row r="172" spans="1:50" ht="24" customHeight="1">
+      <c r="B172" s="13" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="162" spans="1:34" ht="24" customHeight="1">
-      <c r="A162" s="9" t="s">
+    <row r="174" spans="1:50" ht="24" customHeight="1">
+      <c r="A174" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="B162" s="9" t="s">
+      <c r="B174" s="9" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="163" spans="1:34" ht="24" customHeight="1">
-      <c r="A163" s="14" t="s">
+    <row r="175" spans="1:50" ht="24" customHeight="1">
+      <c r="A175" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B163" s="10" t="s">
+      <c r="B175" s="10" t="s">
         <v>599</v>
       </c>
-      <c r="C163" s="10" t="s">
+      <c r="C175" s="10" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="164" spans="1:34" ht="24" customHeight="1">
-      <c r="B164" s="10" t="s">
+    <row r="176" spans="1:50" ht="24" customHeight="1">
+      <c r="B176" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="165" spans="1:34" ht="24" customHeight="1">
-      <c r="B165" s="11"/>
-      <c r="AA165" s="6" t="s">
+    <row r="177" spans="1:34" ht="24" customHeight="1">
+      <c r="B177" s="11"/>
+      <c r="AA177" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="AB165" s="6" t="s">
+      <c r="AB177" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="AC165" s="6" t="s">
+      <c r="AC177" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="AD165" s="6" t="s">
+      <c r="AD177" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="AE165" s="6" t="s">
+      <c r="AE177" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="AF165" s="6" t="s">
+      <c r="AF177" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="AG165" s="6" t="s">
+      <c r="AG177" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="AH165" s="6" t="s">
+      <c r="AH177" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="167" spans="1:34" ht="24" customHeight="1">
-      <c r="A167" s="9" t="s">
+    <row r="179" spans="1:34" ht="24" customHeight="1">
+      <c r="A179" s="9" t="s">
         <v>601</v>
       </c>
-      <c r="B167" s="9" t="s">
+      <c r="B179" s="9" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="168" spans="1:34" ht="24" customHeight="1">
-      <c r="A168" s="14" t="s">
+    <row r="180" spans="1:34" ht="24" customHeight="1">
+      <c r="A180" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B168" s="10" t="s">
+      <c r="B180" s="10" t="s">
         <v>602</v>
       </c>
-      <c r="C168" s="10" t="s">
+      <c r="C180" s="10" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="169" spans="1:34" ht="24" customHeight="1">
-      <c r="B169" s="10" t="s">
+    <row r="181" spans="1:34" ht="24" customHeight="1">
+      <c r="B181" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="170" spans="1:34" ht="24" customHeight="1">
-      <c r="B170" s="11"/>
-      <c r="AA170" s="6" t="s">
+    <row r="182" spans="1:34" ht="24" customHeight="1">
+      <c r="B182" s="11"/>
+      <c r="AA182" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="AB170" s="6" t="s">
+      <c r="AB182" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="AC170" s="6" t="s">
+      <c r="AC182" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="AD170" s="6" t="s">
+      <c r="AD182" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="AE170" s="6" t="s">
+      <c r="AE182" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="AF170" s="6" t="s">
+      <c r="AF182" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="173" spans="1:34" ht="24" customHeight="1">
-      <c r="A173" s="12" t="s">
+    <row r="185" spans="1:34" ht="24" customHeight="1">
+      <c r="A185" s="12" t="s">
         <v>604</v>
       </c>
-      <c r="B173" s="12" t="s">
+      <c r="B185" s="12" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="174" spans="1:34" ht="24" customHeight="1">
-      <c r="B174" s="13" t="s">
+    <row r="186" spans="1:34" ht="24" customHeight="1">
+      <c r="B186" s="13" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="176" spans="1:34" ht="24" customHeight="1">
-      <c r="A176" s="9" t="s">
+    <row r="188" spans="1:34" ht="24" customHeight="1">
+      <c r="A188" s="9" t="s">
         <v>607</v>
       </c>
-      <c r="B176" s="9" t="s">
+      <c r="B188" s="9" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="177" spans="1:31" ht="24" customHeight="1">
-      <c r="A177" s="14" t="s">
+    <row r="189" spans="1:34" ht="24" customHeight="1">
+      <c r="A189" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B177" s="10" t="s">
+      <c r="B189" s="10" t="s">
         <v>608</v>
       </c>
-      <c r="C177" s="10" t="s">
+      <c r="C189" s="10" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="178" spans="1:31" ht="24" customHeight="1">
-      <c r="B178" s="10" t="s">
+    <row r="190" spans="1:34" ht="24" customHeight="1">
+      <c r="B190" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="1:31" ht="24" customHeight="1">
-      <c r="B179" s="11"/>
-      <c r="AA179" s="6" t="s">
+    <row r="191" spans="1:34" ht="24" customHeight="1">
+      <c r="B191" s="11"/>
+      <c r="AA191" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="AB179" s="6" t="s">
+      <c r="AB191" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="AC179" s="6" t="s">
+      <c r="AC191" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="AD179" s="6" t="s">
+      <c r="AD191" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="AE179" s="6" t="s">
+      <c r="AE191" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="181" spans="1:31" ht="24" customHeight="1">
-      <c r="A181" s="9" t="s">
+    <row r="193" spans="1:30" ht="24" customHeight="1">
+      <c r="A193" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="B181" s="9" t="s">
+      <c r="B193" s="9" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="182" spans="1:31" ht="24" customHeight="1">
-      <c r="A182" s="14" t="s">
+    <row r="194" spans="1:30" ht="24" customHeight="1">
+      <c r="A194" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B182" s="10" t="s">
+      <c r="B194" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="C182" s="10" t="s">
+      <c r="C194" s="10" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="183" spans="1:31" ht="24" customHeight="1">
-      <c r="B183" s="10" t="s">
+    <row r="195" spans="1:30" ht="24" customHeight="1">
+      <c r="B195" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="184" spans="1:31" ht="24" customHeight="1">
-      <c r="B184" s="11"/>
-      <c r="AA184" s="6" t="s">
+    <row r="196" spans="1:30" ht="24" customHeight="1">
+      <c r="B196" s="11"/>
+      <c r="AA196" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="AB184" s="6" t="s">
+      <c r="AB196" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="AC184" s="6" t="s">
+      <c r="AC196" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="187" spans="1:31" ht="24" customHeight="1">
-      <c r="A187" s="12" t="s">
+    <row r="199" spans="1:30" ht="24" customHeight="1">
+      <c r="A199" s="12" t="s">
         <v>613</v>
       </c>
-      <c r="B187" s="12" t="s">
+      <c r="B199" s="12" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="188" spans="1:31" ht="24" customHeight="1">
-      <c r="B188" s="13" t="s">
+    <row r="200" spans="1:30" ht="24" customHeight="1">
+      <c r="B200" s="13" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="190" spans="1:31" ht="24" customHeight="1">
-      <c r="A190" s="9" t="s">
+    <row r="202" spans="1:30" ht="24" customHeight="1">
+      <c r="A202" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="B190" s="9" t="s">
+      <c r="B202" s="9" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="191" spans="1:31" ht="24" customHeight="1">
-      <c r="A191" s="14" t="s">
+    <row r="203" spans="1:30" ht="24" customHeight="1">
+      <c r="A203" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B191" s="10" t="s">
+      <c r="B203" s="10" t="s">
         <v>545</v>
       </c>
-      <c r="C191" s="10" t="s">
+      <c r="C203" s="10" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="192" spans="1:31" ht="24" customHeight="1">
-      <c r="B192" s="11"/>
-      <c r="AA192" s="6" t="s">
+    <row r="204" spans="1:30" ht="24" customHeight="1">
+      <c r="B204" s="11"/>
+      <c r="AA204" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="AB192" s="6" t="s">
+      <c r="AB204" s="6" t="s">
         <v>548</v>
       </c>
-      <c r="AC192" s="6" t="s">
+      <c r="AC204" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="AD192" s="6" t="s">
+      <c r="AD204" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="195" spans="1:33" ht="24" customHeight="1">
-      <c r="A195" s="12" t="s">
+    <row r="207" spans="1:30" ht="24" customHeight="1">
+      <c r="A207" s="12" t="s">
         <v>618</v>
       </c>
-      <c r="B195" s="12" t="s">
+      <c r="B207" s="12" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="196" spans="1:33" ht="24" customHeight="1">
-      <c r="B196" s="13" t="s">
+    <row r="208" spans="1:30" ht="24" customHeight="1">
+      <c r="B208" s="13" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="198" spans="1:33" ht="24" customHeight="1">
-      <c r="A198" s="9" t="s">
+    <row r="210" spans="1:33" ht="24" customHeight="1">
+      <c r="A210" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="B198" s="9" t="s">
+      <c r="B210" s="9" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="199" spans="1:33" ht="24" customHeight="1">
-      <c r="A199" s="14" t="s">
+    <row r="211" spans="1:33" ht="24" customHeight="1">
+      <c r="A211" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B199" s="10" t="s">
+      <c r="B211" s="10" t="s">
         <v>622</v>
       </c>
-      <c r="C199" s="10" t="s">
+      <c r="C211" s="10" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="200" spans="1:33" ht="24" customHeight="1">
-      <c r="B200" s="10" t="s">
+    <row r="212" spans="1:33" ht="24" customHeight="1">
+      <c r="B212" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="201" spans="1:33" ht="24" customHeight="1">
-      <c r="B201" s="11"/>
-      <c r="AA201" s="6" t="s">
+    <row r="213" spans="1:33" ht="24" customHeight="1">
+      <c r="B213" s="11"/>
+      <c r="AA213" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="AB201" s="6" t="s">
+      <c r="AB213" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="AC201" s="6" t="s">
+      <c r="AC213" s="6" t="s">
         <v>558</v>
       </c>
-      <c r="AD201" s="6" t="s">
+      <c r="AD213" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="AE201" s="6" t="s">
+      <c r="AE213" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="AF201" s="6" t="s">
+      <c r="AF213" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="AG201" s="6" t="s">
+      <c r="AG213" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="203" spans="1:33" ht="24" customHeight="1">
-      <c r="A203" s="9" t="s">
+    <row r="215" spans="1:33" ht="24" customHeight="1">
+      <c r="A215" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="B203" s="9" t="s">
+      <c r="B215" s="9" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="204" spans="1:33" ht="24" customHeight="1">
-      <c r="A204" s="14" t="s">
+    <row r="216" spans="1:33" ht="24" customHeight="1">
+      <c r="A216" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B204" s="10" t="s">
+      <c r="B216" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="C204" s="10" t="s">
+      <c r="C216" s="10" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="205" spans="1:33" ht="24" customHeight="1">
-      <c r="B205" s="10" t="s">
+    <row r="217" spans="1:33" ht="24" customHeight="1">
+      <c r="B217" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="206" spans="1:33" ht="24" customHeight="1">
-      <c r="B206" s="11"/>
-      <c r="AA206" s="6" t="s">
+    <row r="218" spans="1:33" ht="24" customHeight="1">
+      <c r="B218" s="11"/>
+      <c r="AA218" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="AB206" s="6" t="s">
+      <c r="AB218" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="AC206" s="6" t="s">
+      <c r="AC218" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="AD206" s="6" t="s">
+      <c r="AD218" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="AE206" s="6" t="s">
+      <c r="AE218" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="AF206" s="6" t="s">
+      <c r="AF218" s="6" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="29">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
-      <formula1>AA16:AN16</formula1>
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32 B204 B131 B105">
+      <formula1>AA32:AD32</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
-      <formula1>AA28:AD28</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37 B218 B182 B136 B119 B83">
+      <formula1>AA37:AF37</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33">
-      <formula1>AA33:AF33</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41 B140">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
-      <formula1>AA42:AC42</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46 B196 B145 B97">
+      <formula1>AA46:AC46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
-      <formula1>AA51:AK51</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55:B59 B154:B158">
+      <formula1>AA55:AK55</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56">
-      <formula1>AA56:AR56</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64 B163">
+      <formula1>AA64:AR64</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61">
-      <formula1>AA61:AX61</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69 B168">
+      <formula1>AA69:AX69</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70">
-      <formula1>AA70:AH70</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78 B177">
+      <formula1>AA78:AH78</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
-      <formula1>AA75:AF75</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92 B191">
+      <formula1>AA92:AE92</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84">
-      <formula1>AA84:AE84</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114 B213">
+      <formula1>AA114:AG114</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">
-      <formula1>AA89:AC89</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B97">
-      <formula1>AA97:AD97</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B106">
-      <formula1>AA106:AG106</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B111">
-      <formula1>AA111:AF111</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B123">
-      <formula1>AA123:AD123</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B128">
-      <formula1>AA128:AF128</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B132">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B137">
-      <formula1>AA137:AC137</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B146">
-      <formula1>AA146:AK146</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B151">
-      <formula1>AA151:AR151</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B156">
-      <formula1>AA156:AX156</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B165">
-      <formula1>AA165:AH165</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B170">
-      <formula1>AA170:AF170</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B179">
-      <formula1>AA179:AE179</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B184">
-      <formula1>AA184:AC184</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B192">
-      <formula1>AA192:AD192</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B201">
-      <formula1>AA201:AG201</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B206">
-      <formula1>AA206:AF206</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B20">
+      <formula1>AA16:AN16</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8565,12 +9201,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK87"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -8637,7 +9275,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -8673,7 +9311,9 @@
       </c>
     </row>
     <row r="19" spans="1:37" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>642</v>
+      </c>
       <c r="AA19" s="6" t="s">
         <v>642</v>
       </c>
@@ -8824,7 +9464,9 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="24" customHeight="1">
-      <c r="B40" s="11"/>
+      <c r="B40" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="42" spans="1:30" ht="24" customHeight="1">
       <c r="A42" s="9" t="s">
@@ -8851,7 +9493,9 @@
       </c>
     </row>
     <row r="45" spans="1:30" ht="24" customHeight="1">
-      <c r="B45" s="11"/>
+      <c r="B45" s="11" t="s">
+        <v>675</v>
+      </c>
       <c r="AA45" s="6" t="s">
         <v>675</v>
       </c>
@@ -9039,7 +9683,9 @@
       </c>
     </row>
     <row r="68" spans="1:30" ht="24" customHeight="1">
-      <c r="B68" s="11"/>
+      <c r="B68" s="11" t="s">
+        <v>1039</v>
+      </c>
     </row>
     <row r="70" spans="1:30" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
@@ -9066,7 +9712,9 @@
       </c>
     </row>
     <row r="73" spans="1:30" ht="24" customHeight="1">
-      <c r="B73" s="11"/>
+      <c r="B73" s="11" t="s">
+        <v>675</v>
+      </c>
       <c r="AA73" s="6" t="s">
         <v>675</v>
       </c>
@@ -9239,12 +9887,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -9285,7 +9935,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1040</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -9311,7 +9963,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -9374,7 +10026,9 @@
       </c>
     </row>
     <row r="24" spans="1:31" ht="24" customHeight="1">
-      <c r="B24" s="11"/>
+      <c r="B24" s="11" t="s">
+        <v>747</v>
+      </c>
       <c r="AA24" s="6" t="s">
         <v>747</v>
       </c>
@@ -9391,102 +10045,164 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="24" customHeight="1">
-      <c r="A27" s="12" t="s">
+    <row r="25" spans="1:31" ht="24" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>748</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AC25" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AE25" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="24.75" customHeight="1">
+      <c r="B26" s="11" t="s">
+        <v>749</v>
+      </c>
+      <c r="AA26" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AB26" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AC26" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AD26" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AE26" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="24.75" customHeight="1">
+      <c r="B27" s="11" t="s">
+        <v>750</v>
+      </c>
+      <c r="AA27" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AB27" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AC27" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AD27" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AE27" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" ht="24" customHeight="1">
+      <c r="A30" s="12" t="s">
         <v>751</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B30" s="12" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="24" customHeight="1">
-      <c r="B28" s="13" t="s">
+    <row r="31" spans="1:31" ht="24" customHeight="1">
+      <c r="B31" s="13" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="24" customHeight="1">
-      <c r="A30" s="9" t="s">
+    <row r="33" spans="1:35" ht="24" customHeight="1">
+      <c r="A33" s="9" t="s">
         <v>754</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="24" customHeight="1">
-      <c r="A31" s="14" t="s">
+    <row r="34" spans="1:35" ht="24" customHeight="1">
+      <c r="A34" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B34" s="10" t="s">
         <v>755</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="24" customHeight="1">
-      <c r="B32" s="11"/>
-    </row>
-    <row r="34" spans="1:35" ht="24" customHeight="1">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:35" ht="24" customHeight="1">
+      <c r="B35" s="11" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" ht="24" customHeight="1">
+      <c r="A37" s="9" t="s">
         <v>757</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="35" spans="1:35" ht="24" customHeight="1">
-      <c r="A35" s="14" t="s">
+    <row r="38" spans="1:35" ht="24" customHeight="1">
+      <c r="A38" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>758</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="24" customHeight="1">
-      <c r="B36" s="10" t="s">
+    <row r="39" spans="1:35" ht="24" customHeight="1">
+      <c r="B39" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="24" customHeight="1">
-      <c r="B37" s="11"/>
-      <c r="AA37" s="6" t="s">
+    <row r="40" spans="1:35" ht="24" customHeight="1">
+      <c r="B40" s="11"/>
+      <c r="AA40" s="6" t="s">
         <v>760</v>
       </c>
-      <c r="AB37" s="6" t="s">
+      <c r="AB40" s="6" t="s">
         <v>761</v>
       </c>
-      <c r="AC37" s="6" t="s">
+      <c r="AC40" s="6" t="s">
         <v>762</v>
       </c>
-      <c r="AD37" s="6" t="s">
+      <c r="AD40" s="6" t="s">
         <v>763</v>
       </c>
-      <c r="AE37" s="6" t="s">
+      <c r="AE40" s="6" t="s">
         <v>764</v>
       </c>
-      <c r="AF37" s="6" t="s">
+      <c r="AF40" s="6" t="s">
         <v>765</v>
       </c>
-      <c r="AG37" s="6" t="s">
+      <c r="AG40" s="6" t="s">
         <v>766</v>
       </c>
-      <c r="AH37" s="6" t="s">
+      <c r="AH40" s="6" t="s">
         <v>767</v>
       </c>
-      <c r="AI37" s="6" t="s">
+      <c r="AI40" s="6" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B27">
       <formula1>AA24:AE24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
-      <formula1>AA37:AI37</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40">
+      <formula1>AA40:AI40</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9494,12 +10210,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH89"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -9566,8 +10284,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+    <row r="11" spans="1:29" ht="177.95" customHeight="1">
+      <c r="B11" s="11" t="s">
+        <v>1041</v>
+      </c>
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">

</xml_diff>